<commit_message>
Metad Data Updated as csv
</commit_message>
<xml_diff>
--- a/Data/test_metadata-free-free-system.xlsx
+++ b/Data/test_metadata-free-free-system.xlsx
@@ -16,18 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>d1</t>
-  </si>
-  <si>
-    <t>d2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>l1</t>
   </si>
   <si>
     <t>l2</t>
+  </si>
+  <si>
+    <t>depth</t>
   </si>
 </sst>
 </file>
@@ -366,445 +363,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.5</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>63</v>
       </c>
       <c r="C2">
-        <v>63</v>
-      </c>
-      <c r="D2">
         <v>510</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>255</v>
       </c>
       <c r="C3">
-        <v>255</v>
-      </c>
-      <c r="D3">
         <v>742</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.5</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>284</v>
       </c>
       <c r="C4">
-        <v>284</v>
-      </c>
-      <c r="D4">
         <v>392</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.5</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>290</v>
       </c>
       <c r="C5">
-        <v>290</v>
-      </c>
-      <c r="D5">
         <v>804</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.5</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>440</v>
       </c>
       <c r="C6">
-        <v>440</v>
-      </c>
-      <c r="D6">
         <v>639</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C7">
-        <v>36</v>
-      </c>
-      <c r="D7">
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="C8">
-        <v>183</v>
-      </c>
-      <c r="D8">
         <v>844</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>535</v>
       </c>
       <c r="C9">
-        <v>535</v>
-      </c>
-      <c r="D9">
         <v>548</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>581</v>
       </c>
       <c r="C10">
-        <v>581</v>
-      </c>
-      <c r="D10">
         <v>699</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>588</v>
       </c>
       <c r="C11">
-        <v>588</v>
-      </c>
-      <c r="D11">
         <v>618</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>35</v>
-      </c>
-      <c r="D12">
         <v>337</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C13">
-        <v>66</v>
-      </c>
-      <c r="D13">
         <v>707</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>252</v>
       </c>
       <c r="C14">
-        <v>252</v>
-      </c>
-      <c r="D14">
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>348</v>
       </c>
       <c r="C15">
-        <v>348</v>
-      </c>
-      <c r="D15">
         <v>684</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>389</v>
       </c>
       <c r="C16">
-        <v>389</v>
-      </c>
-      <c r="D16">
         <v>834</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C17">
-        <v>154</v>
-      </c>
-      <c r="D17">
         <v>844</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>168</v>
       </c>
       <c r="C18">
-        <v>168</v>
-      </c>
-      <c r="D18">
         <v>497</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C19">
-        <v>183</v>
-      </c>
-      <c r="D19">
         <v>562</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>369</v>
       </c>
       <c r="C20">
-        <v>369</v>
-      </c>
-      <c r="D20">
         <v>942</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>579</v>
       </c>
       <c r="C21">
-        <v>579</v>
-      </c>
-      <c r="D21">
         <v>826</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C22">
-        <v>69</v>
-      </c>
-      <c r="D22">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="C23">
-        <v>108</v>
-      </c>
-      <c r="D23">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>198</v>
       </c>
       <c r="C24">
-        <v>198</v>
-      </c>
-      <c r="D24">
         <v>439</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>428</v>
       </c>
       <c r="C25">
-        <v>428</v>
-      </c>
-      <c r="D25">
         <v>907</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>516</v>
       </c>
       <c r="C26">
-        <v>516</v>
-      </c>
-      <c r="D26">
         <v>719</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>257</v>
       </c>
       <c r="C27">
-        <v>257</v>
-      </c>
-      <c r="D27">
         <v>933</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>330</v>
       </c>
       <c r="C28">
-        <v>330</v>
-      </c>
-      <c r="D28">
         <v>346</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>566</v>
       </c>
       <c r="C29">
-        <v>566</v>
-      </c>
-      <c r="D29">
         <v>804</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>648</v>
       </c>
       <c r="C30">
-        <v>648</v>
-      </c>
-      <c r="D30">
         <v>814</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>697</v>
       </c>
       <c r="C31">
-        <v>697</v>
-      </c>
-      <c r="D31">
         <v>953</v>
       </c>
     </row>
@@ -813,7 +717,6 @@
     <sortCondition ref="A2:A31"/>
     <sortCondition ref="B2:B31"/>
     <sortCondition ref="C2:C31"/>
-    <sortCondition ref="D2:D31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>